<commit_message>
created new stored procedure for new order demand prediction
</commit_message>
<xml_diff>
--- a/database/ezoom_db_objects.xlsx
+++ b/database/ezoom_db_objects.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20904"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DD101E1-6221-4B9E-81D3-E328D7CAC5F5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="179020" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="262">
   <si>
     <t>object type</t>
   </si>
@@ -33,51 +34,87 @@
     <t>Note</t>
   </si>
   <si>
+    <t>stored procedure</t>
+  </si>
+  <si>
     <t>add_attribute_to_product</t>
   </si>
   <si>
-    <t>stored procedure</t>
+    <t>procedure for add_attribute_to_product</t>
   </si>
   <si>
     <t>add_ingredient_to_recipe</t>
   </si>
   <si>
+    <t>procedure for add_ingredient_to_recipe</t>
+  </si>
+  <si>
     <t>add_step_to_process</t>
   </si>
   <si>
+    <t>procedure for add_step_to_process</t>
+  </si>
+  <si>
     <t>alt_dc_column</t>
   </si>
   <si>
+    <t>procedure for altering data columns</t>
+  </si>
+  <si>
     <t>associate_product_process</t>
   </si>
   <si>
+    <t>procedure for associating a process with a product</t>
+  </si>
+  <si>
     <t>autoload_client</t>
   </si>
   <si>
+    <t>procedure for autoloading clients</t>
+  </si>
+  <si>
     <t>used when load vendors/customers from Quickbooks export file</t>
   </si>
   <si>
     <t>autoload_inventory</t>
   </si>
   <si>
+    <t>procedure for autoloading inventory</t>
+  </si>
+  <si>
     <t>autoload_material</t>
   </si>
   <si>
+    <t>procedure for autoloading material</t>
+  </si>
+  <si>
     <t>check_approver</t>
   </si>
   <si>
+    <t>approval procedure</t>
+  </si>
+  <si>
+    <t>check_emp_access</t>
+  </si>
+  <si>
+    <t>procedure for checking employee access</t>
+  </si>
+  <si>
+    <t>consume_inventory</t>
+  </si>
+  <si>
+    <t>procedure for creating consume_inventory</t>
+  </si>
+  <si>
     <t>function</t>
   </si>
   <si>
-    <t>check_emp_access</t>
-  </si>
-  <si>
-    <t>consume_inventory</t>
-  </si>
-  <si>
     <t>convert_quantity</t>
   </si>
   <si>
+    <t>function for converting quantity</t>
+  </si>
+  <si>
     <t>table</t>
   </si>
   <si>
@@ -120,33 +157,6 @@
     <t>create_dc_data_general</t>
   </si>
   <si>
-    <t>procedure for associating a process with a product</t>
-  </si>
-  <si>
-    <t>procedure for autoloading clients</t>
-  </si>
-  <si>
-    <t>procedure for autoloading inventory</t>
-  </si>
-  <si>
-    <t>procedure for altering data columns</t>
-  </si>
-  <si>
-    <t>procedure for autoloading material</t>
-  </si>
-  <si>
-    <t>approval procedure</t>
-  </si>
-  <si>
-    <t>procedure for checking employee access</t>
-  </si>
-  <si>
-    <t>procedure for creating consume_inventory</t>
-  </si>
-  <si>
-    <t>function for converting quantity</t>
-  </si>
-  <si>
     <t>dc_data_general table</t>
   </si>
   <si>
@@ -180,24 +190,15 @@
     <t>employee_group table</t>
   </si>
   <si>
-    <t>procedure for add_attribute_to_product</t>
-  </si>
-  <si>
-    <t>procedure for add_ingredient_to_recipe</t>
-  </si>
-  <si>
-    <t>procedure for add_step_to_process</t>
-  </si>
-  <si>
     <t>create_eq_attributes</t>
   </si>
   <si>
+    <t>eq_attributes table</t>
+  </si>
+  <si>
     <t>create_equip_history</t>
   </si>
   <si>
-    <t>eq_attributes table</t>
-  </si>
-  <si>
     <t>equip_history table</t>
   </si>
   <si>
@@ -279,12 +280,12 @@
     <t>material_supplier table</t>
   </si>
   <si>
+    <t>create_order</t>
+  </si>
+  <si>
     <t>order table</t>
   </si>
   <si>
-    <t>create_order</t>
-  </si>
-  <si>
     <t>create_order_detail</t>
   </si>
   <si>
@@ -375,12 +376,12 @@
     <t>recipe table</t>
   </si>
   <si>
+    <t>Create_Role_Table</t>
+  </si>
+  <si>
     <t>system_roles table</t>
   </si>
   <si>
-    <t>Create_Role_Table</t>
-  </si>
-  <si>
     <t>create_step</t>
   </si>
   <si>
@@ -408,15 +409,15 @@
     <t>delete_equipment</t>
   </si>
   <si>
+    <t>procedure for deleting equipment</t>
+  </si>
+  <si>
     <t>delete_material</t>
   </si>
   <si>
     <t>procedure for deleting material</t>
   </si>
   <si>
-    <t>procedure for deleting equipment</t>
-  </si>
-  <si>
     <t>delete_order</t>
   </si>
   <si>
@@ -687,12 +688,12 @@
     <t>report_consumption_for_step</t>
   </si>
   <si>
+    <t>procedure outputing the consumption information for a given lot/batch and given step</t>
+  </si>
+  <si>
     <t>report_dispatch_history</t>
   </si>
   <si>
-    <t>procedure outputing the consumption information for a given lot/batch and given step</t>
-  </si>
-  <si>
     <t>procedure for reporting dispatch history</t>
   </si>
   <si>
@@ -759,12 +760,12 @@
     <t>select_lot_info_for_start_step</t>
   </si>
   <si>
+    <t>procedure for selecting lot info for starting step</t>
+  </si>
+  <si>
     <t>select_step_details</t>
   </si>
   <si>
-    <t>procedure for selecting lot info for starting step</t>
-  </si>
-  <si>
     <t>procedure for selecting step details</t>
   </si>
   <si>
@@ -780,10 +781,16 @@
     <t>procedure for starting lot step</t>
   </si>
   <si>
+    <t>new_order_demand_prediction</t>
+  </si>
+  <si>
+    <t>procedure that get new order demand prediction</t>
+  </si>
+  <si>
+    <t>view</t>
+  </si>
+  <si>
     <t>view_ingredient</t>
-  </si>
-  <si>
-    <t>view</t>
   </si>
   <si>
     <t>view for ingredient</t>
@@ -804,7 +811,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="12"/>
@@ -853,6 +860,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1177,11 +1192,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D126"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D127"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C126" sqref="C126"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1208,288 +1223,288 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>54</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B23" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>56</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C27" t="s">
         <v>59</v>
@@ -1497,7 +1512,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
         <v>60</v>
@@ -1508,7 +1523,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>62</v>
@@ -1519,7 +1534,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>64</v>
@@ -1530,7 +1545,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>66</v>
@@ -1541,7 +1556,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>68</v>
@@ -1552,7 +1567,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>70</v>
@@ -1563,7 +1578,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
         <v>72</v>
@@ -1574,7 +1589,7 @@
     </row>
     <row r="35" spans="1:3">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B35" t="s">
         <v>74</v>
@@ -1585,7 +1600,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B36" t="s">
         <v>76</v>
@@ -1596,7 +1611,7 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B37" t="s">
         <v>78</v>
@@ -1607,7 +1622,7 @@
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
         <v>80</v>
@@ -1618,7 +1633,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B39" t="s">
         <v>82</v>
@@ -1629,7 +1644,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
         <v>84</v>
@@ -1640,18 +1655,18 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" t="s">
         <v>87</v>
-      </c>
-      <c r="C41" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B42" t="s">
         <v>88</v>
@@ -1662,7 +1677,7 @@
     </row>
     <row r="43" spans="1:3">
       <c r="A43" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B43" t="s">
         <v>90</v>
@@ -1673,7 +1688,7 @@
     </row>
     <row r="44" spans="1:3">
       <c r="A44" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B44" t="s">
         <v>92</v>
@@ -1684,7 +1699,7 @@
     </row>
     <row r="45" spans="1:3">
       <c r="A45" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B45" t="s">
         <v>94</v>
@@ -1695,7 +1710,7 @@
     </row>
     <row r="46" spans="1:3">
       <c r="A46" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B46" t="s">
         <v>96</v>
@@ -1706,7 +1721,7 @@
     </row>
     <row r="47" spans="1:3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B47" t="s">
         <v>98</v>
@@ -1717,7 +1732,7 @@
     </row>
     <row r="48" spans="1:3">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B48" t="s">
         <v>100</v>
@@ -1728,7 +1743,7 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
         <v>102</v>
@@ -1739,7 +1754,7 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B50" t="s">
         <v>104</v>
@@ -1750,7 +1765,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B51" t="s">
         <v>106</v>
@@ -1761,7 +1776,7 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B52" t="s">
         <v>108</v>
@@ -1772,7 +1787,7 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
         <v>110</v>
@@ -1783,7 +1798,7 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B54" t="s">
         <v>112</v>
@@ -1794,7 +1809,7 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B55" t="s">
         <v>114</v>
@@ -1805,7 +1820,7 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B56" t="s">
         <v>116</v>
@@ -1816,18 +1831,18 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B57" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" t="s">
         <v>119</v>
-      </c>
-      <c r="C57" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B58" t="s">
         <v>120</v>
@@ -1838,7 +1853,7 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B59" t="s">
         <v>122</v>
@@ -1849,7 +1864,7 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B60" t="s">
         <v>124</v>
@@ -1860,7 +1875,7 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B61" t="s">
         <v>126</v>
@@ -1871,29 +1886,29 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B62" t="s">
         <v>128</v>
       </c>
       <c r="C62" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B64" t="s">
         <v>132</v>
@@ -1907,7 +1922,7 @@
     </row>
     <row r="65" spans="1:3">
       <c r="A65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B65" t="s">
         <v>135</v>
@@ -1918,7 +1933,7 @@
     </row>
     <row r="66" spans="1:3">
       <c r="A66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B66" t="s">
         <v>137</v>
@@ -1929,7 +1944,7 @@
     </row>
     <row r="67" spans="1:3">
       <c r="A67" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B67" t="s">
         <v>139</v>
@@ -1940,7 +1955,7 @@
     </row>
     <row r="68" spans="1:3">
       <c r="A68" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B68" t="s">
         <v>141</v>
@@ -1951,7 +1966,7 @@
     </row>
     <row r="69" spans="1:3">
       <c r="A69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B69" t="s">
         <v>143</v>
@@ -1962,7 +1977,7 @@
     </row>
     <row r="70" spans="1:3">
       <c r="A70" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B70" t="s">
         <v>145</v>
@@ -1973,7 +1988,7 @@
     </row>
     <row r="71" spans="1:3">
       <c r="A71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
         <v>147</v>
@@ -1984,7 +1999,7 @@
     </row>
     <row r="72" spans="1:3">
       <c r="A72" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B72" t="s">
         <v>149</v>
@@ -1995,7 +2010,7 @@
     </row>
     <row r="73" spans="1:3">
       <c r="A73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B73" t="s">
         <v>151</v>
@@ -2006,7 +2021,7 @@
     </row>
     <row r="74" spans="1:3">
       <c r="A74" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="B74" t="s">
         <v>153</v>
@@ -2017,7 +2032,7 @@
     </row>
     <row r="75" spans="1:3">
       <c r="A75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B75" t="s">
         <v>155</v>
@@ -2028,7 +2043,7 @@
     </row>
     <row r="76" spans="1:3">
       <c r="A76" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B76" t="s">
         <v>157</v>
@@ -2039,7 +2054,7 @@
     </row>
     <row r="77" spans="1:3">
       <c r="A77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B77" t="s">
         <v>159</v>
@@ -2050,7 +2065,7 @@
     </row>
     <row r="78" spans="1:3">
       <c r="A78" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B78" t="s">
         <v>161</v>
@@ -2061,7 +2076,7 @@
     </row>
     <row r="79" spans="1:3">
       <c r="A79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B79" t="s">
         <v>163</v>
@@ -2072,7 +2087,7 @@
     </row>
     <row r="80" spans="1:3">
       <c r="A80" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B80" t="s">
         <v>165</v>
@@ -2083,7 +2098,7 @@
     </row>
     <row r="81" spans="1:3">
       <c r="A81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B81" t="s">
         <v>167</v>
@@ -2094,7 +2109,7 @@
     </row>
     <row r="82" spans="1:3">
       <c r="A82" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B82" t="s">
         <v>169</v>
@@ -2105,7 +2120,7 @@
     </row>
     <row r="83" spans="1:3">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B83" t="s">
         <v>171</v>
@@ -2116,7 +2131,7 @@
     </row>
     <row r="84" spans="1:3">
       <c r="A84" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B84" t="s">
         <v>173</v>
@@ -2127,7 +2142,7 @@
     </row>
     <row r="85" spans="1:3">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B85" t="s">
         <v>175</v>
@@ -2138,7 +2153,7 @@
     </row>
     <row r="86" spans="1:3">
       <c r="A86" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B86" t="s">
         <v>177</v>
@@ -2149,7 +2164,7 @@
     </row>
     <row r="87" spans="1:3">
       <c r="A87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B87" t="s">
         <v>179</v>
@@ -2160,7 +2175,7 @@
     </row>
     <row r="88" spans="1:3">
       <c r="A88" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B88" t="s">
         <v>181</v>
@@ -2171,7 +2186,7 @@
     </row>
     <row r="89" spans="1:3">
       <c r="A89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B89" t="s">
         <v>183</v>
@@ -2182,7 +2197,7 @@
     </row>
     <row r="90" spans="1:3">
       <c r="A90" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B90" t="s">
         <v>185</v>
@@ -2193,7 +2208,7 @@
     </row>
     <row r="91" spans="1:3">
       <c r="A91" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B91" t="s">
         <v>187</v>
@@ -2204,7 +2219,7 @@
     </row>
     <row r="92" spans="1:3">
       <c r="A92" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B92" t="s">
         <v>189</v>
@@ -2215,7 +2230,7 @@
     </row>
     <row r="93" spans="1:3">
       <c r="A93" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B93" t="s">
         <v>191</v>
@@ -2226,7 +2241,7 @@
     </row>
     <row r="94" spans="1:3">
       <c r="A94" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B94" t="s">
         <v>193</v>
@@ -2237,7 +2252,7 @@
     </row>
     <row r="95" spans="1:3">
       <c r="A95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B95" t="s">
         <v>195</v>
@@ -2248,7 +2263,7 @@
     </row>
     <row r="96" spans="1:3">
       <c r="A96" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B96" t="s">
         <v>197</v>
@@ -2259,7 +2274,7 @@
     </row>
     <row r="97" spans="1:3">
       <c r="A97" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B97" t="s">
         <v>199</v>
@@ -2270,7 +2285,7 @@
     </row>
     <row r="98" spans="1:3">
       <c r="A98" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B98" t="s">
         <v>201</v>
@@ -2281,7 +2296,7 @@
     </row>
     <row r="99" spans="1:3">
       <c r="A99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B99" t="s">
         <v>203</v>
@@ -2292,7 +2307,7 @@
     </row>
     <row r="100" spans="1:3">
       <c r="A100" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B100" t="s">
         <v>205</v>
@@ -2303,7 +2318,7 @@
     </row>
     <row r="101" spans="1:3">
       <c r="A101" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B101" t="s">
         <v>207</v>
@@ -2314,7 +2329,7 @@
     </row>
     <row r="102" spans="1:3">
       <c r="A102" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B102" t="s">
         <v>209</v>
@@ -2325,7 +2340,7 @@
     </row>
     <row r="103" spans="1:3">
       <c r="A103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B103" t="s">
         <v>211</v>
@@ -2336,7 +2351,7 @@
     </row>
     <row r="104" spans="1:3">
       <c r="A104" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B104" t="s">
         <v>213</v>
@@ -2347,7 +2362,7 @@
     </row>
     <row r="105" spans="1:3">
       <c r="A105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B105" t="s">
         <v>215</v>
@@ -2358,7 +2373,7 @@
     </row>
     <row r="106" spans="1:3">
       <c r="A106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B106" t="s">
         <v>217</v>
@@ -2369,7 +2384,7 @@
     </row>
     <row r="107" spans="1:3">
       <c r="A107" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B107" t="s">
         <v>219</v>
@@ -2380,21 +2395,21 @@
     </row>
     <row r="108" spans="1:3">
       <c r="A108" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B108" t="s">
         <v>221</v>
       </c>
       <c r="C108" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="109" spans="1:3">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C109" t="s">
         <v>224</v>
@@ -2402,7 +2417,7 @@
     </row>
     <row r="110" spans="1:3">
       <c r="A110" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B110" t="s">
         <v>225</v>
@@ -2413,7 +2428,7 @@
     </row>
     <row r="111" spans="1:3">
       <c r="A111" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B111" t="s">
         <v>227</v>
@@ -2424,7 +2439,7 @@
     </row>
     <row r="112" spans="1:3">
       <c r="A112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B112" t="s">
         <v>229</v>
@@ -2435,7 +2450,7 @@
     </row>
     <row r="113" spans="1:3">
       <c r="A113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B113" t="s">
         <v>231</v>
@@ -2446,7 +2461,7 @@
     </row>
     <row r="114" spans="1:3">
       <c r="A114" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B114" t="s">
         <v>233</v>
@@ -2457,7 +2472,7 @@
     </row>
     <row r="115" spans="1:3">
       <c r="A115" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B115" t="s">
         <v>235</v>
@@ -2468,7 +2483,7 @@
     </row>
     <row r="116" spans="1:3">
       <c r="A116" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B116" t="s">
         <v>237</v>
@@ -2479,7 +2494,7 @@
     </row>
     <row r="117" spans="1:3">
       <c r="A117" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B117" t="s">
         <v>239</v>
@@ -2490,7 +2505,7 @@
     </row>
     <row r="118" spans="1:3">
       <c r="A118" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B118" t="s">
         <v>241</v>
@@ -2501,7 +2516,7 @@
     </row>
     <row r="119" spans="1:3">
       <c r="A119" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B119" t="s">
         <v>243</v>
@@ -2512,21 +2527,21 @@
     </row>
     <row r="120" spans="1:3">
       <c r="A120" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B120" t="s">
         <v>245</v>
       </c>
       <c r="C120" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="121" spans="1:3">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B121" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C121" t="s">
         <v>248</v>
@@ -2534,7 +2549,7 @@
     </row>
     <row r="122" spans="1:3">
       <c r="A122" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B122" t="s">
         <v>249</v>
@@ -2545,7 +2560,7 @@
     </row>
     <row r="123" spans="1:3">
       <c r="A123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B123" t="s">
         <v>251</v>
@@ -2556,18 +2571,18 @@
     </row>
     <row r="124" spans="1:3">
       <c r="A124" t="s">
-        <v>254</v>
+        <v>4</v>
       </c>
       <c r="B124" t="s">
         <v>253</v>
       </c>
       <c r="C124" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B125" t="s">
         <v>256</v>
@@ -2578,7 +2593,7 @@
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B126" t="s">
         <v>258</v>
@@ -2587,9 +2602,20 @@
         <v>259</v>
       </c>
     </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>255</v>
+      </c>
+      <c r="B127" t="s">
+        <v>260</v>
+      </c>
+      <c r="C127" t="s">
+        <v>261</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"table,stored procedure,function,view,type"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
fixed bugs in new_order_demand_prediction and updated order_dispatch_display_per_product.sql and updated load_procedures and ezoom_db_objects.xlsx
</commit_message>
<xml_diff>
--- a/database/ezoom_db_objects.xlsx
+++ b/database/ezoom_db_objects.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20904"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6DD101E1-6221-4B9E-81D3-E328D7CAC5F5}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5144510-679C-45B3-ADC1-C1B821C13206}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="264">
   <si>
     <t>object type</t>
   </si>
@@ -785,6 +785,12 @@
   </si>
   <si>
     <t>procedure that get new order demand prediction</t>
+  </si>
+  <si>
+    <t>order_dispatch_display_per_product.sql</t>
+  </si>
+  <si>
+    <t>dispatch product per order and predict max final product allowed by inventory</t>
   </si>
   <si>
     <t>view</t>
@@ -1193,10 +1199,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D127"/>
+  <dimension ref="A1:D128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C124" sqref="C124"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2582,18 +2588,18 @@
     </row>
     <row r="125" spans="1:3">
       <c r="A125" t="s">
+        <v>4</v>
+      </c>
+      <c r="B125" t="s">
         <v>255</v>
       </c>
-      <c r="B125" t="s">
+      <c r="C125" t="s">
         <v>256</v>
-      </c>
-      <c r="C125" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B126" t="s">
         <v>258</v>
@@ -2604,13 +2610,24 @@
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B127" t="s">
         <v>260</v>
       </c>
       <c r="C127" t="s">
         <v>261</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>257</v>
+      </c>
+      <c r="B128" t="s">
+        <v>262</v>
+      </c>
+      <c r="C128" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
record new sp in db object list file
</commit_message>
<xml_diff>
--- a/database/ezoom_db_objects.xlsx
+++ b/database/ezoom_db_objects.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20904"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5144510-679C-45B3-ADC1-C1B821C13206}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="266">
   <si>
     <t>object type</t>
   </si>
@@ -812,13 +811,19 @@
   </si>
   <si>
     <t>view for process step</t>
+  </si>
+  <si>
+    <t>modify_product_group</t>
+  </si>
+  <si>
+    <t>procedure for inserting or modifying product group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1198,22 +1203,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D128"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C131" sqref="C131"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.625" customWidth="1"/>
-    <col min="3" max="3" width="43.125" customWidth="1"/>
+    <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="43.1640625" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="21">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="20">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2371,10 +2376,10 @@
         <v>4</v>
       </c>
       <c r="B105" t="s">
-        <v>215</v>
+        <v>264</v>
       </c>
       <c r="C105" t="s">
-        <v>216</v>
+        <v>265</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2382,10 +2387,10 @@
         <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C106" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2393,10 +2398,10 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C107" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2404,10 +2409,10 @@
         <v>4</v>
       </c>
       <c r="B108" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C108" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2415,10 +2420,10 @@
         <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C109" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2426,10 +2431,10 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C110" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2437,10 +2442,10 @@
         <v>4</v>
       </c>
       <c r="B111" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C111" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2448,10 +2453,10 @@
         <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C112" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2459,10 +2464,10 @@
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C113" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2470,10 +2475,10 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2481,10 +2486,10 @@
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C115" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2492,10 +2497,10 @@
         <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C116" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2503,10 +2508,10 @@
         <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C117" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2514,10 +2519,10 @@
         <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C118" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2525,10 +2530,10 @@
         <v>4</v>
       </c>
       <c r="B119" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C119" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2536,10 +2541,10 @@
         <v>4</v>
       </c>
       <c r="B120" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C120" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2547,10 +2552,10 @@
         <v>4</v>
       </c>
       <c r="B121" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="C121" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2558,10 +2563,10 @@
         <v>4</v>
       </c>
       <c r="B122" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C122" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2569,10 +2574,10 @@
         <v>4</v>
       </c>
       <c r="B123" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="C123" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2580,10 +2585,10 @@
         <v>4</v>
       </c>
       <c r="B124" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C124" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2591,21 +2596,21 @@
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C125" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="126" spans="1:3">
       <c r="A126" t="s">
-        <v>257</v>
+        <v>4</v>
       </c>
       <c r="B126" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="C126" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="127" spans="1:3">
@@ -2613,10 +2618,10 @@
         <v>257</v>
       </c>
       <c r="B127" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="C127" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="128" spans="1:3">
@@ -2624,15 +2629,26 @@
         <v>257</v>
       </c>
       <c r="B128" t="s">
+        <v>260</v>
+      </c>
+      <c r="C128" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>257</v>
+      </c>
+      <c r="B129" t="s">
         <v>262</v>
       </c>
-      <c r="C128" t="s">
+      <c r="C129" t="s">
         <v>263</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
       <formula1>"table,stored procedure,function,view,type"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated ezoom_db_objects.xlsx and load_procedures.sql
</commit_message>
<xml_diff>
--- a/database/ezoom_db_objects.xlsx
+++ b/database/ezoom_db_objects.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21015"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E3D027F-7A9B-46A1-996F-820673A0D496}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="179020" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="268">
   <si>
     <t>object type</t>
   </si>
@@ -666,6 +672,12 @@
     <t>procedure for modifying uom</t>
   </si>
   <si>
+    <t>modify_product_group</t>
+  </si>
+  <si>
+    <t>procedure for inserting or modifying product group</t>
+  </si>
+  <si>
     <t>pass_lot_step</t>
   </si>
   <si>
@@ -792,6 +804,12 @@
     <t>dispatch product per order and predict max final product allowed by inventory</t>
   </si>
   <si>
+    <t>relocate_inventory</t>
+  </si>
+  <si>
+    <t>relocate items from one location to a new location, depending on destination, either resulting in a merge into existed record (same item, destination, serial no of parent/descendant) or creating a new record</t>
+  </si>
+  <si>
     <t>view</t>
   </si>
   <si>
@@ -811,19 +829,13 @@
   </si>
   <si>
     <t>view for process step</t>
-  </si>
-  <si>
-    <t>modify_product_group</t>
-  </si>
-  <si>
-    <t>procedure for inserting or modifying product group</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1203,22 +1215,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D129"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <selection activeCell="C132" sqref="C132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="43.1640625" customWidth="1"/>
+    <col min="2" max="2" width="32.625" customWidth="1"/>
+    <col min="3" max="3" width="43.125" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="20.100000000000001">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2376,10 +2388,10 @@
         <v>4</v>
       </c>
       <c r="B105" t="s">
-        <v>264</v>
+        <v>215</v>
       </c>
       <c r="C105" t="s">
-        <v>265</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:3">
@@ -2387,10 +2399,10 @@
         <v>4</v>
       </c>
       <c r="B106" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C106" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="107" spans="1:3">
@@ -2398,10 +2410,10 @@
         <v>4</v>
       </c>
       <c r="B107" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C107" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="108" spans="1:3">
@@ -2409,10 +2421,10 @@
         <v>4</v>
       </c>
       <c r="B108" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="C108" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
     </row>
     <row r="109" spans="1:3">
@@ -2420,10 +2432,10 @@
         <v>4</v>
       </c>
       <c r="B109" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="C109" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="110" spans="1:3">
@@ -2431,10 +2443,10 @@
         <v>4</v>
       </c>
       <c r="B110" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="C110" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="111" spans="1:3">
@@ -2442,10 +2454,10 @@
         <v>4</v>
       </c>
       <c r="B111" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C111" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="112" spans="1:3">
@@ -2453,10 +2465,10 @@
         <v>4</v>
       </c>
       <c r="B112" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C112" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="113" spans="1:3">
@@ -2464,10 +2476,10 @@
         <v>4</v>
       </c>
       <c r="B113" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C113" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:3">
@@ -2475,10 +2487,10 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="C114" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="115" spans="1:3">
@@ -2486,10 +2498,10 @@
         <v>4</v>
       </c>
       <c r="B115" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="C115" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="116" spans="1:3">
@@ -2497,10 +2509,10 @@
         <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="C116" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="117" spans="1:3">
@@ -2508,10 +2520,10 @@
         <v>4</v>
       </c>
       <c r="B117" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C117" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
     </row>
     <row r="118" spans="1:3">
@@ -2519,10 +2531,10 @@
         <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="C118" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="119" spans="1:3">
@@ -2530,10 +2542,10 @@
         <v>4</v>
       </c>
       <c r="B119" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="C119" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -2541,10 +2553,10 @@
         <v>4</v>
       </c>
       <c r="B120" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="C120" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="121" spans="1:3">
@@ -2552,10 +2564,10 @@
         <v>4</v>
       </c>
       <c r="B121" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="C121" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
     </row>
     <row r="122" spans="1:3">
@@ -2563,10 +2575,10 @@
         <v>4</v>
       </c>
       <c r="B122" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C122" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
     </row>
     <row r="123" spans="1:3">
@@ -2574,10 +2586,10 @@
         <v>4</v>
       </c>
       <c r="B123" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="C123" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="124" spans="1:3">
@@ -2585,10 +2597,10 @@
         <v>4</v>
       </c>
       <c r="B124" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C124" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row r="125" spans="1:3">
@@ -2596,10 +2608,10 @@
         <v>4</v>
       </c>
       <c r="B125" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C125" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
     </row>
     <row r="126" spans="1:3">
@@ -2607,48 +2619,59 @@
         <v>4</v>
       </c>
       <c r="B126" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="C126" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="127" spans="1:3">
       <c r="A127" t="s">
-        <v>257</v>
+        <v>4</v>
       </c>
       <c r="B127" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C127" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="128" spans="1:3">
       <c r="A128" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B128" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C128" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row r="129" spans="1:3">
       <c r="A129" t="s">
-        <v>257</v>
+        <v>261</v>
       </c>
       <c r="B129" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C129" t="s">
-        <v>263</v>
+        <v>265</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>261</v>
+      </c>
+      <c r="B130" t="s">
+        <v>266</v>
+      </c>
+      <c r="C130" t="s">
+        <v>267</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"table,stored procedure,function,view,type"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
created modify_location and update accordingly
</commit_message>
<xml_diff>
--- a/database/ezoom_db_objects.xlsx
+++ b/database/ezoom_db_objects.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E3D027F-7A9B-46A1-996F-820673A0D496}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ITHelps\ezoom_newrepo\database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A69A4E-9EEA-46D7-889D-D413419BE776}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8730" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179020" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="270">
   <si>
     <t>object type</t>
   </si>
@@ -829,13 +829,19 @@
   </si>
   <si>
     <t>view for process step</t>
+  </si>
+  <si>
+    <t>modify_location</t>
+  </si>
+  <si>
+    <t>validate user's inputs, insert a new location or update an old one</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1216,21 +1222,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D130"/>
+  <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="C132" sqref="C132"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="24.5" customWidth="1"/>
-    <col min="2" max="2" width="32.625" customWidth="1"/>
-    <col min="3" max="3" width="43.125" customWidth="1"/>
+    <col min="2" max="2" width="32.59765625" customWidth="1"/>
+    <col min="3" max="3" width="43.09765625" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="20.100000000000001">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1255,7 +1261,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1277,7 +1283,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1294,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1299,7 +1305,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1313,7 +1319,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -1335,7 +1341,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -1346,7 +1352,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1368,7 +1374,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -1379,7 +1385,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1390,7 +1396,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1401,7 +1407,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1412,7 +1418,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -1423,7 +1429,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A18" t="s">
         <v>31</v>
       </c>
@@ -1434,7 +1440,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -1445,7 +1451,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1456,7 +1462,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1467,7 +1473,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -1500,7 +1506,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1511,7 +1517,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1522,7 +1528,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -1533,7 +1539,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A28" t="s">
         <v>31</v>
       </c>
@@ -1544,7 +1550,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1555,7 +1561,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1566,7 +1572,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -1577,7 +1583,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1588,7 +1594,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1610,7 +1616,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -1621,7 +1627,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1632,7 +1638,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A37" t="s">
         <v>31</v>
       </c>
@@ -1643,7 +1649,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A38" t="s">
         <v>31</v>
       </c>
@@ -1654,7 +1660,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1665,7 +1671,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A40" t="s">
         <v>31</v>
       </c>
@@ -1676,7 +1682,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A41" t="s">
         <v>31</v>
       </c>
@@ -1687,7 +1693,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A42" t="s">
         <v>31</v>
       </c>
@@ -1698,7 +1704,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A44" t="s">
         <v>31</v>
       </c>
@@ -1720,7 +1726,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -1731,7 +1737,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A46" t="s">
         <v>31</v>
       </c>
@@ -1742,7 +1748,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -1753,7 +1759,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A48" t="s">
         <v>31</v>
       </c>
@@ -1764,7 +1770,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A49" t="s">
         <v>31</v>
       </c>
@@ -1775,7 +1781,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A50" t="s">
         <v>31</v>
       </c>
@@ -1786,7 +1792,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A51" t="s">
         <v>31</v>
       </c>
@@ -1797,7 +1803,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A52" t="s">
         <v>31</v>
       </c>
@@ -1808,7 +1814,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A53" t="s">
         <v>31</v>
       </c>
@@ -1819,7 +1825,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A54" t="s">
         <v>31</v>
       </c>
@@ -1830,7 +1836,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A55" t="s">
         <v>31</v>
       </c>
@@ -1841,7 +1847,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -1852,7 +1858,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A57" t="s">
         <v>31</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A58" t="s">
         <v>31</v>
       </c>
@@ -1874,7 +1880,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -1885,7 +1891,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -1896,7 +1902,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -1907,7 +1913,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A62" t="s">
         <v>4</v>
       </c>
@@ -1918,7 +1924,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.6">
       <c r="A64" t="s">
         <v>4</v>
       </c>
@@ -1943,7 +1949,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A65" t="s">
         <v>4</v>
       </c>
@@ -1954,7 +1960,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A66" t="s">
         <v>4</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A67" t="s">
         <v>4</v>
       </c>
@@ -1976,7 +1982,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A68" t="s">
         <v>4</v>
       </c>
@@ -1987,7 +1993,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A69" t="s">
         <v>4</v>
       </c>
@@ -1998,7 +2004,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A70" t="s">
         <v>4</v>
       </c>
@@ -2009,7 +2015,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A71" t="s">
         <v>4</v>
       </c>
@@ -2020,7 +2026,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A72" t="s">
         <v>4</v>
       </c>
@@ -2031,7 +2037,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A73" t="s">
         <v>4</v>
       </c>
@@ -2042,7 +2048,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A74" t="s">
         <v>28</v>
       </c>
@@ -2053,7 +2059,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A75" t="s">
         <v>4</v>
       </c>
@@ -2064,7 +2070,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A76" t="s">
         <v>4</v>
       </c>
@@ -2075,7 +2081,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A77" t="s">
         <v>4</v>
       </c>
@@ -2086,7 +2092,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A78" t="s">
         <v>4</v>
       </c>
@@ -2097,7 +2103,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A79" t="s">
         <v>4</v>
       </c>
@@ -2108,7 +2114,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A80" t="s">
         <v>4</v>
       </c>
@@ -2119,7 +2125,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A81" t="s">
         <v>4</v>
       </c>
@@ -2130,7 +2136,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A82" t="s">
         <v>4</v>
       </c>
@@ -2141,7 +2147,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A83" t="s">
         <v>4</v>
       </c>
@@ -2152,7 +2158,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A84" t="s">
         <v>4</v>
       </c>
@@ -2163,7 +2169,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A85" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2180,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A86" t="s">
         <v>31</v>
       </c>
@@ -2185,7 +2191,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A87" t="s">
         <v>4</v>
       </c>
@@ -2196,7 +2202,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A88" t="s">
         <v>4</v>
       </c>
@@ -2207,7 +2213,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A89" t="s">
         <v>4</v>
       </c>
@@ -2218,7 +2224,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A90" t="s">
         <v>4</v>
       </c>
@@ -2229,7 +2235,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A91" t="s">
         <v>4</v>
       </c>
@@ -2240,7 +2246,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A92" t="s">
         <v>4</v>
       </c>
@@ -2251,7 +2257,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A93" t="s">
         <v>4</v>
       </c>
@@ -2262,7 +2268,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A94" t="s">
         <v>4</v>
       </c>
@@ -2273,7 +2279,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A95" t="s">
         <v>4</v>
       </c>
@@ -2284,7 +2290,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A96" t="s">
         <v>4</v>
       </c>
@@ -2295,7 +2301,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A97" t="s">
         <v>4</v>
       </c>
@@ -2306,7 +2312,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A98" t="s">
         <v>4</v>
       </c>
@@ -2317,7 +2323,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A99" t="s">
         <v>4</v>
       </c>
@@ -2328,7 +2334,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A100" t="s">
         <v>4</v>
       </c>
@@ -2339,7 +2345,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A101" t="s">
         <v>4</v>
       </c>
@@ -2350,7 +2356,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A102" t="s">
         <v>4</v>
       </c>
@@ -2361,7 +2367,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A103" t="s">
         <v>4</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A104" t="s">
         <v>4</v>
       </c>
@@ -2383,7 +2389,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A105" t="s">
         <v>4</v>
       </c>
@@ -2394,7 +2400,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A106" t="s">
         <v>4</v>
       </c>
@@ -2405,7 +2411,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A107" t="s">
         <v>4</v>
       </c>
@@ -2416,7 +2422,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A108" t="s">
         <v>4</v>
       </c>
@@ -2427,7 +2433,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A109" t="s">
         <v>4</v>
       </c>
@@ -2438,7 +2444,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A110" t="s">
         <v>4</v>
       </c>
@@ -2449,7 +2455,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A111" t="s">
         <v>4</v>
       </c>
@@ -2460,7 +2466,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A112" t="s">
         <v>4</v>
       </c>
@@ -2471,7 +2477,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A113" t="s">
         <v>4</v>
       </c>
@@ -2482,7 +2488,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A114" t="s">
         <v>4</v>
       </c>
@@ -2493,7 +2499,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A115" t="s">
         <v>4</v>
       </c>
@@ -2504,7 +2510,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A116" t="s">
         <v>4</v>
       </c>
@@ -2515,7 +2521,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A117" t="s">
         <v>4</v>
       </c>
@@ -2526,7 +2532,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A118" t="s">
         <v>4</v>
       </c>
@@ -2537,7 +2543,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A119" t="s">
         <v>4</v>
       </c>
@@ -2548,7 +2554,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A120" t="s">
         <v>4</v>
       </c>
@@ -2559,7 +2565,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A121" t="s">
         <v>4</v>
       </c>
@@ -2570,7 +2576,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A122" t="s">
         <v>4</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A123" t="s">
         <v>4</v>
       </c>
@@ -2592,7 +2598,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A124" t="s">
         <v>4</v>
       </c>
@@ -2603,7 +2609,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A125" t="s">
         <v>4</v>
       </c>
@@ -2614,7 +2620,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A126" t="s">
         <v>4</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A127" t="s">
         <v>4</v>
       </c>
@@ -2636,36 +2642,47 @@
         <v>260</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A128" t="s">
-        <v>261</v>
+        <v>4</v>
       </c>
       <c r="B128" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="C128" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="129" spans="1:3">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A129" t="s">
         <v>261</v>
       </c>
       <c r="B129" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C129" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="130" spans="1:3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A130" t="s">
         <v>261</v>
       </c>
       <c r="B130" t="s">
+        <v>264</v>
+      </c>
+      <c r="C130" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A131" t="s">
+        <v>261</v>
+      </c>
+      <c r="B131" t="s">
         <v>266</v>
       </c>
-      <c r="C130" t="s">
+      <c r="C131" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new sp report_order and update files accordingly
</commit_message>
<xml_diff>
--- a/database/ezoom_db_objects.xlsx
+++ b/database/ezoom_db_objects.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ITHelps\ezoom_newrepo\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A69A4E-9EEA-46D7-889D-D413419BE776}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89031767-81D4-4C2F-BE6C-DAA302D0FFFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8730" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179020" concurrentCalc="0"/>
+  <calcPr calcId="179020"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="272">
   <si>
     <t>object type</t>
   </si>
@@ -835,6 +835,12 @@
   </si>
   <si>
     <t>validate user's inputs, insert a new location or update an old one</t>
+  </si>
+  <si>
+    <t>report_order</t>
+  </si>
+  <si>
+    <t>input an order_id, product_id, lot_status, shows lot information</t>
   </si>
 </sst>
 </file>
@@ -1222,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D131"/>
+  <dimension ref="A1:D132"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -2655,13 +2661,13 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.6">
       <c r="A129" t="s">
-        <v>261</v>
+        <v>4</v>
       </c>
       <c r="B129" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="C129" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.6">
@@ -2669,10 +2675,10 @@
         <v>261</v>
       </c>
       <c r="B130" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C130" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.6">
@@ -2680,9 +2686,20 @@
         <v>261</v>
       </c>
       <c r="B131" t="s">
+        <v>264</v>
+      </c>
+      <c r="C131" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A132" t="s">
+        <v>261</v>
+      </c>
+      <c r="B132" t="s">
         <v>266</v>
       </c>
-      <c r="C131" t="s">
+      <c r="C132" t="s">
         <v>267</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added new stored procedure orderconsumptioninventoryreport
</commit_message>
<xml_diff>
--- a/database/ezoom_db_objects.xlsx
+++ b/database/ezoom_db_objects.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\ITHelps\ezoom_newrepo\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89031767-81D4-4C2F-BE6C-DAA302D0FFFF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE182CF7-2BA0-4B56-BA16-E6BD84628CD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8730" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3078" yWindow="1176" windowWidth="19512" windowHeight="11184" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="274">
   <si>
     <t>object type</t>
   </si>
@@ -841,6 +841,12 @@
   </si>
   <si>
     <t>input an order_id, product_id, lot_status, shows lot information</t>
+  </si>
+  <si>
+    <t>order_consumption_inventory_report</t>
+  </si>
+  <si>
+    <t>stored procedure for checking any ongoing batches that are at step 8 (consumption material step) in open orders</t>
   </si>
 </sst>
 </file>
@@ -1228,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D132"/>
+  <dimension ref="A1:D133"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A123" workbookViewId="0">
+      <selection activeCell="D135" sqref="D135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -2701,6 +2707,17 @@
       </c>
       <c r="C132" t="s">
         <v>267</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.6">
+      <c r="A133" t="s">
+        <v>4</v>
+      </c>
+      <c r="B133" t="s">
+        <v>272</v>
+      </c>
+      <c r="C133" t="s">
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>